<commit_message>
update recovery on D1 added D2
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GS03FLMA_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GS03FLMA_00001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\# OOI_Asset_Management\GS_mod\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="456" windowWidth="25356" windowHeight="15816" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="450" windowWidth="25350" windowHeight="15810"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -1387,30 +1387,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.44140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="8.77734375" style="4"/>
+    <col min="8" max="8" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="8.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>86</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -1467,7 +1467,9 @@
       <c r="F2" s="12">
         <v>0.99652777777777779</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="7">
+        <v>42345</v>
+      </c>
       <c r="H2" s="3" t="s">
         <v>51</v>
       </c>
@@ -1490,7 +1492,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
       <c r="G3" s="17"/>
@@ -1510,25 +1512,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="2" customWidth="1"/>
     <col min="7" max="7" width="27" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.77734375" style="2"/>
+    <col min="8" max="8" width="22.140625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="23" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="23" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1557,7 +1559,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>58</v>
       </c>
@@ -1586,7 +1588,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>58</v>
       </c>
@@ -1615,7 +1617,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>58</v>
       </c>
@@ -1641,7 +1643,7 @@
         <v>1.21E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>58</v>
       </c>
@@ -1667,7 +1669,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>58</v>
       </c>
@@ -1693,7 +1695,7 @@
         <v>9.0499999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>58</v>
       </c>
@@ -1719,7 +1721,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>58</v>
       </c>
@@ -1748,7 +1750,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>58</v>
       </c>
@@ -1777,7 +1779,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>58</v>
       </c>
@@ -1806,7 +1808,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>58</v>
       </c>
@@ -1835,7 +1837,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12"/>
       <c r="C12" s="13"/>
@@ -1845,7 +1847,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>72</v>
       </c>
@@ -1874,7 +1876,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>72</v>
       </c>
@@ -1900,7 +1902,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>72</v>
       </c>
@@ -1926,7 +1928,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>72</v>
       </c>
@@ -1952,7 +1954,7 @@
         <v>38502</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>72</v>
       </c>
@@ -1978,7 +1980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>72</v>
       </c>
@@ -2004,7 +2006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>72</v>
       </c>
@@ -2033,7 +2035,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20"/>
       <c r="C20" s="13"/>
@@ -2043,7 +2045,7 @@
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>48</v>
       </c>
@@ -2072,7 +2074,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>48</v>
       </c>
@@ -2101,7 +2103,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>48</v>
       </c>
@@ -2127,7 +2129,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24"/>
       <c r="C24" s="13"/>
@@ -2137,7 +2139,7 @@
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>59</v>
       </c>
@@ -2166,7 +2168,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>59</v>
       </c>
@@ -2192,7 +2194,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>59</v>
       </c>
@@ -2218,7 +2220,7 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>59</v>
       </c>
@@ -2244,7 +2246,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>59</v>
       </c>
@@ -2270,7 +2272,7 @@
         <v>500000</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>59</v>
       </c>
@@ -2296,7 +2298,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>59</v>
       </c>
@@ -2322,7 +2324,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>59</v>
       </c>
@@ -2348,7 +2350,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>59</v>
       </c>
@@ -2374,7 +2376,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="13"/>
       <c r="B34"/>
       <c r="C34" s="13"/>
@@ -2384,7 +2386,7 @@
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
     </row>
-    <row r="35" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>60</v>
       </c>
@@ -2413,7 +2415,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>60</v>
       </c>
@@ -2439,7 +2441,7 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>60</v>
       </c>
@@ -2465,7 +2467,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>60</v>
       </c>
@@ -2491,7 +2493,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39"/>
       <c r="C39" s="13"/>
@@ -2501,7 +2503,7 @@
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
     </row>
-    <row r="40" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>61</v>
       </c>
@@ -2530,7 +2532,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>61</v>
       </c>
@@ -2556,7 +2558,7 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>61</v>
       </c>
@@ -2582,7 +2584,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>61</v>
       </c>
@@ -2608,7 +2610,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44"/>
       <c r="C44" s="13"/>
@@ -2618,7 +2620,7 @@
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
     </row>
-    <row r="45" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>62</v>
       </c>
@@ -2647,7 +2649,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>62</v>
       </c>
@@ -2673,7 +2675,7 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>62</v>
       </c>
@@ -2699,7 +2701,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>62</v>
       </c>
@@ -2725,7 +2727,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
       <c r="B49"/>
       <c r="C49" s="13"/>
@@ -2735,7 +2737,7 @@
       <c r="G49" s="13"/>
       <c r="H49" s="13"/>
     </row>
-    <row r="50" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>63</v>
       </c>
@@ -2764,7 +2766,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>63</v>
       </c>
@@ -2790,7 +2792,7 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="13" t="s">
         <v>63</v>
       </c>
@@ -2816,7 +2818,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>63</v>
       </c>
@@ -2842,7 +2844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="13"/>
       <c r="B54"/>
       <c r="C54" s="13"/>
@@ -2852,7 +2854,7 @@
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
     </row>
-    <row r="55" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="13" t="s">
         <v>64</v>
       </c>
@@ -2881,7 +2883,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
         <v>64</v>
       </c>
@@ -2907,7 +2909,7 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="13" t="s">
         <v>64</v>
       </c>
@@ -2933,7 +2935,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="13" t="s">
         <v>64</v>
       </c>
@@ -2959,7 +2961,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="13"/>
       <c r="B59"/>
       <c r="C59" s="13"/>
@@ -2969,7 +2971,7 @@
       <c r="G59" s="13"/>
       <c r="H59" s="13"/>
     </row>
-    <row r="60" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
         <v>65</v>
       </c>
@@ -2998,7 +3000,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="13" t="s">
         <v>65</v>
       </c>
@@ -3024,7 +3026,7 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="13" t="s">
         <v>65</v>
       </c>
@@ -3050,7 +3052,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="13" t="s">
         <v>65</v>
       </c>
@@ -3076,7 +3078,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="13"/>
       <c r="B64"/>
       <c r="C64" s="13"/>
@@ -3086,7 +3088,7 @@
       <c r="G64" s="13"/>
       <c r="H64" s="13"/>
     </row>
-    <row r="65" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="13" t="s">
         <v>66</v>
       </c>
@@ -3115,7 +3117,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="13" t="s">
         <v>66</v>
       </c>
@@ -3141,7 +3143,7 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="13" t="s">
         <v>66</v>
       </c>
@@ -3167,7 +3169,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="13" t="s">
         <v>66</v>
       </c>
@@ -3193,7 +3195,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69"/>
       <c r="C69" s="13"/>
@@ -3203,7 +3205,7 @@
       <c r="G69" s="13"/>
       <c r="H69" s="13"/>
     </row>
-    <row r="70" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="13" t="s">
         <v>67</v>
       </c>
@@ -3232,7 +3234,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="13" t="s">
         <v>67</v>
       </c>
@@ -3258,7 +3260,7 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="13" t="s">
         <v>67</v>
       </c>
@@ -3284,7 +3286,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
         <v>67</v>
       </c>
@@ -3310,7 +3312,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
       <c r="B74"/>
       <c r="C74" s="13"/>
@@ -3320,7 +3322,7 @@
       <c r="G74" s="13"/>
       <c r="H74" s="13"/>
     </row>
-    <row r="75" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
         <v>68</v>
       </c>
@@ -3349,7 +3351,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="13" t="s">
         <v>68</v>
       </c>
@@ -3375,7 +3377,7 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="13" t="s">
         <v>68</v>
       </c>
@@ -3401,7 +3403,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>68</v>
       </c>
@@ -3427,7 +3429,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="13"/>
       <c r="B79"/>
       <c r="C79" s="13"/>
@@ -3437,7 +3439,7 @@
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
     </row>
-    <row r="80" spans="1:9" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>69</v>
       </c>
@@ -3466,7 +3468,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>69</v>
       </c>
@@ -3492,7 +3494,7 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>69</v>
       </c>
@@ -3518,7 +3520,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>69</v>
       </c>
@@ -3544,7 +3546,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="13"/>
       <c r="B84"/>
       <c r="C84" s="13"/>
@@ -3554,7 +3556,7 @@
       <c r="G84" s="13"/>
       <c r="H84" s="13"/>
     </row>
-    <row r="85" spans="1:9" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>70</v>
       </c>
@@ -3583,7 +3585,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>70</v>
       </c>
@@ -3609,7 +3611,7 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>70</v>
       </c>
@@ -3635,7 +3637,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>70</v>
       </c>
@@ -3661,7 +3663,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="13"/>
       <c r="B89"/>
       <c r="C89" s="13"/>
@@ -3671,7 +3673,7 @@
       <c r="G89" s="13"/>
       <c r="H89" s="13"/>
     </row>
-    <row r="90" spans="1:9" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>71</v>
       </c>
@@ -3700,7 +3702,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>71</v>
       </c>
@@ -3726,7 +3728,7 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>71</v>
       </c>
@@ -3752,7 +3754,7 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>71</v>
       </c>
@@ -3778,7 +3780,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
       <c r="B94"/>
       <c r="C94" s="13"/>
@@ -3788,7 +3790,7 @@
       <c r="G94" s="13"/>
       <c r="H94" s="13"/>
     </row>
-    <row r="95" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
         <v>50</v>
       </c>
@@ -3811,7 +3813,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="13"/>
       <c r="B96" s="13"/>
       <c r="C96" s="13"/>
@@ -3821,7 +3823,7 @@
       <c r="G96" s="13"/>
       <c r="H96" s="13"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="13"/>
       <c r="B97" s="13"/>
       <c r="C97" s="13"/>
@@ -3831,7 +3833,7 @@
       <c r="G97" s="13"/>
       <c r="H97" s="13"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="13"/>
       <c r="B98" s="13"/>
       <c r="C98" s="13"/>
@@ -3841,7 +3843,7 @@
       <c r="G98" s="13"/>
       <c r="H98" s="13"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="13"/>
       <c r="B99" s="13"/>
       <c r="C99" s="13"/>
@@ -3851,7 +3853,7 @@
       <c r="G99" s="13"/>
       <c r="H99" s="13"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="13"/>
       <c r="B100" s="13"/>
       <c r="C100" s="13"/>
@@ -3861,7 +3863,7 @@
       <c r="G100" s="13"/>
       <c r="H100" s="13"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="13"/>
       <c r="B101" s="13"/>
       <c r="C101" s="13"/>

</xml_diff>

<commit_message>
Corrected CTD reference designators, added D2 Integration CSV
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GS03FLMA_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GS03FLMA_00001.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="450" windowWidth="25350" windowHeight="15810"/>
+    <workbookView xWindow="720" yWindow="450" windowWidth="25350" windowHeight="15810" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="109">
   <si>
     <t>Ref Des</t>
   </si>
@@ -184,9 +184,6 @@
     <t>Requires TEMPWAT, PRESWAT, and PRACSAL from GS03FLMA-RIS02-03-CTDMOG000</t>
   </si>
   <si>
-    <t>GS03FLMA-FM001-00-ENG000000</t>
-  </si>
-  <si>
     <t>54° 06.31' S</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
     <t>[2.847181E-03,1.209779E-04,2.411834E-06,2.302539E+02,-3.288590E-01,-5.735673E+01,4.554631E+00]</t>
   </si>
   <si>
-    <t>GS03FLMA-00001-ENG</t>
-  </si>
-  <si>
     <t>The serial number used here is bogus, pending identification of the real serial number.</t>
   </si>
   <si>
@@ -212,42 +206,6 @@
   </si>
   <si>
     <t>GS03FLMA-RIM01-02-ADCPSL003</t>
-  </si>
-  <si>
-    <t>GS03FLMA-RIM01-02-CTDMOG088</t>
-  </si>
-  <si>
-    <t>GS03FLMA-RIM01-02-CTDMOG030</t>
-  </si>
-  <si>
-    <t>GS03FLMA-RIM01-02-CTDMOG076</t>
-  </si>
-  <si>
-    <t>GS03FLMA-RIM01-02-CTDMOG071</t>
-  </si>
-  <si>
-    <t>GS03FLMA-RIM01-02-CTDMOG074</t>
-  </si>
-  <si>
-    <t>GS03FLMA-RIM01-02-CTDMOG036</t>
-  </si>
-  <si>
-    <t>GS03FLMA-RIM01-02-CTDMOG072</t>
-  </si>
-  <si>
-    <t>GS03FLMA-RIM01-02-CTDMOG033</t>
-  </si>
-  <si>
-    <t>GS03FLMA-RIM01-02-CTDMOG070</t>
-  </si>
-  <si>
-    <t>GS03FLMA-RIM01-02-CTDMOH085</t>
-  </si>
-  <si>
-    <t>GS03FLMA-RIM01-02-CTDMOH091</t>
-  </si>
-  <si>
-    <t>GS03FLMA-RIM01-02-CTDMOH090</t>
   </si>
   <si>
     <t>GS03FLMA-RIS01-04-PHSENF000</t>
@@ -368,6 +326,60 @@
   </si>
   <si>
     <t>A00961</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIS01-00-SIOENG000</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIM01-02-CTDMOG040</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIM01-02-CTDMOG041</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIM01-02-CTDMOG042</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIM01-02-CTDMOG043</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIM01-02-CTDMOG044</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIM01-02-CTDMOG045</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIM01-02-CTDMOG046</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIM01-02-CTDMOG047</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIM01-02-CTDMOG048</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIM01-02-CTDMOH049</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIM01-02-CTDMOH050</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIM01-02-CTDMOH051</t>
+  </si>
+  <si>
+    <t>GS03FLMA-RIM01-00-SIOENG000</t>
+  </si>
+  <si>
+    <t>GS03FLMA-00001-ENG- main</t>
+  </si>
+  <si>
+    <t>GS03FLMA-00001-ENG-sec</t>
+  </si>
+  <si>
+    <t>OL000247</t>
+  </si>
+  <si>
+    <t>OL000248</t>
   </si>
 </sst>
 </file>
@@ -1387,8 +1399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1412,7 +1424,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>0</v>
@@ -1450,10 +1462,10 @@
     </row>
     <row r="2" spans="1:14" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>47</v>
@@ -1471,16 +1483,16 @@
         <v>42345</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="J2" s="26">
         <v>4632</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="11">
@@ -1510,10 +1522,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="G102" sqref="G102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1527,7 +1539,9 @@
     <col min="7" max="7" width="27" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.7109375" style="2"/>
+    <col min="10" max="14" width="8.7109375" style="2"/>
+    <col min="15" max="15" width="12" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="23" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
@@ -1535,7 +1549,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>1</v>
@@ -1544,7 +1558,7 @@
         <v>41</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="F1" s="22" t="s">
         <v>2</v>
@@ -1561,10 +1575,10 @@
     </row>
     <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>47</v>
@@ -1573,7 +1587,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F2" s="13">
         <v>1216</v>
@@ -1590,10 +1604,10 @@
     </row>
     <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>47</v>
@@ -1602,7 +1616,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F3" s="13">
         <v>1216</v>
@@ -1619,10 +1633,10 @@
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>47</v>
@@ -1631,7 +1645,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F4" s="13">
         <v>1216</v>
@@ -1645,10 +1659,10 @@
     </row>
     <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>47</v>
@@ -1657,7 +1671,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F5" s="13">
         <v>1216</v>
@@ -1671,10 +1685,10 @@
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>47</v>
@@ -1683,7 +1697,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F6" s="13">
         <v>1216</v>
@@ -1697,10 +1711,10 @@
     </row>
     <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>47</v>
@@ -1709,7 +1723,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F7" s="13">
         <v>1216</v>
@@ -1723,10 +1737,10 @@
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>47</v>
@@ -1735,7 +1749,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F8" s="13">
         <v>1216</v>
@@ -1752,10 +1766,10 @@
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>47</v>
@@ -1764,7 +1778,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F9" s="13">
         <v>1216</v>
@@ -1781,10 +1795,10 @@
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>47</v>
@@ -1793,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F10" s="13">
         <v>1216</v>
@@ -1810,10 +1824,10 @@
     </row>
     <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>47</v>
@@ -1822,7 +1836,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="F11" s="13">
         <v>1216</v>
@@ -1849,10 +1863,10 @@
     </row>
     <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>47</v>
@@ -1861,10 +1875,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>18</v>
@@ -1878,10 +1892,10 @@
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>47</v>
@@ -1890,10 +1904,10 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>19</v>
@@ -1904,10 +1918,10 @@
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>47</v>
@@ -1916,10 +1930,10 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>20</v>
@@ -1930,10 +1944,10 @@
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>47</v>
@@ -1942,10 +1956,10 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>21</v>
@@ -1956,10 +1970,10 @@
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>47</v>
@@ -1968,10 +1982,10 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>22</v>
@@ -1982,10 +1996,10 @@
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>47</v>
@@ -1994,10 +2008,10 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>23</v>
@@ -2008,10 +2022,10 @@
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>47</v>
@@ -2020,10 +2034,10 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>39</v>
@@ -2050,7 +2064,7 @@
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>47</v>
@@ -2059,7 +2073,7 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F21" s="13">
         <v>393</v>
@@ -2079,7 +2093,7 @@
         <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>47</v>
@@ -2088,7 +2102,7 @@
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F22" s="13">
         <v>393</v>
@@ -2108,7 +2122,7 @@
         <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>47</v>
@@ -2117,7 +2131,7 @@
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F23" s="13">
         <v>393</v>
@@ -2126,7 +2140,7 @@
         <v>15</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -2141,10 +2155,10 @@
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>47</v>
@@ -2153,7 +2167,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F25" s="13">
         <v>18352</v>
@@ -2170,10 +2184,10 @@
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>47</v>
@@ -2182,7 +2196,7 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F26" s="13">
         <v>18352</v>
@@ -2196,10 +2210,10 @@
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>47</v>
@@ -2208,7 +2222,7 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F27" s="13">
         <v>18352</v>
@@ -2222,10 +2236,10 @@
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>47</v>
@@ -2234,7 +2248,7 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F28" s="13">
         <v>18352</v>
@@ -2248,10 +2262,10 @@
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>47</v>
@@ -2260,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F29" s="13">
         <v>18352</v>
@@ -2274,10 +2288,10 @@
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>47</v>
@@ -2286,7 +2300,7 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F30" s="13">
         <v>18352</v>
@@ -2300,10 +2314,10 @@
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>47</v>
@@ -2312,7 +2326,7 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F31" s="13">
         <v>18352</v>
@@ -2326,10 +2340,10 @@
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>47</v>
@@ -2338,7 +2352,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F32" s="13">
         <v>18352</v>
@@ -2352,10 +2366,10 @@
     </row>
     <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>47</v>
@@ -2364,7 +2378,7 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="F33" s="13">
         <v>18352</v>
@@ -2387,23 +2401,23 @@
       <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="14">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="24" t="s">
         <v>60</v>
-      </c>
-      <c r="B35" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" s="14">
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
-        <v>93</v>
-      </c>
-      <c r="F35" s="24" t="s">
-        <v>74</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>5</v>
@@ -2416,23 +2430,23 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="14">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="24" t="s">
         <v>60</v>
-      </c>
-      <c r="B36" t="s">
-        <v>88</v>
-      </c>
-      <c r="C36" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D36" s="14">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
-        <v>93</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>74</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>6</v>
@@ -2442,23 +2456,23 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="14">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>79</v>
+      </c>
+      <c r="F37" s="24" t="s">
         <v>60</v>
-      </c>
-      <c r="B37" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="14">
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>93</v>
-      </c>
-      <c r="F37" s="24" t="s">
-        <v>74</v>
       </c>
       <c r="G37" s="13" t="s">
         <v>7</v>
@@ -2468,23 +2482,23 @@
       </c>
     </row>
     <row r="38" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" s="14">
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="24" t="s">
         <v>60</v>
-      </c>
-      <c r="B38" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="14">
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>93</v>
-      </c>
-      <c r="F38" s="24" t="s">
-        <v>74</v>
       </c>
       <c r="G38" s="13" t="s">
         <v>29</v>
@@ -2504,23 +2518,23 @@
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="14">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>80</v>
+      </c>
+      <c r="F40" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="B40" t="s">
-        <v>88</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="14">
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
-        <v>94</v>
-      </c>
-      <c r="F40" s="24" t="s">
-        <v>75</v>
       </c>
       <c r="G40" s="13" t="s">
         <v>5</v>
@@ -2533,23 +2547,23 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="14">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>80</v>
+      </c>
+      <c r="F41" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="B41" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="14">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
-        <v>94</v>
-      </c>
-      <c r="F41" s="24" t="s">
-        <v>75</v>
       </c>
       <c r="G41" s="13" t="s">
         <v>6</v>
@@ -2559,23 +2573,23 @@
       </c>
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="14">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>80</v>
+      </c>
+      <c r="F42" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="B42" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="14">
-        <v>1</v>
-      </c>
-      <c r="E42" t="s">
-        <v>94</v>
-      </c>
-      <c r="F42" s="24" t="s">
-        <v>75</v>
       </c>
       <c r="G42" s="13" t="s">
         <v>7</v>
@@ -2585,23 +2599,23 @@
       </c>
     </row>
     <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="14">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>80</v>
+      </c>
+      <c r="F43" s="24" t="s">
         <v>61</v>
-      </c>
-      <c r="B43" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="14">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>94</v>
-      </c>
-      <c r="F43" s="24" t="s">
-        <v>75</v>
       </c>
       <c r="G43" s="13" t="s">
         <v>29</v>
@@ -2621,23 +2635,23 @@
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" s="14">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>81</v>
+      </c>
+      <c r="F45" s="24" t="s">
         <v>62</v>
-      </c>
-      <c r="B45" t="s">
-        <v>88</v>
-      </c>
-      <c r="C45" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D45" s="14">
-        <v>1</v>
-      </c>
-      <c r="E45" t="s">
-        <v>95</v>
-      </c>
-      <c r="F45" s="24" t="s">
-        <v>76</v>
       </c>
       <c r="G45" s="13" t="s">
         <v>5</v>
@@ -2650,23 +2664,23 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="14">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>81</v>
+      </c>
+      <c r="F46" s="24" t="s">
         <v>62</v>
-      </c>
-      <c r="B46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D46" s="14">
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
-        <v>95</v>
-      </c>
-      <c r="F46" s="24" t="s">
-        <v>76</v>
       </c>
       <c r="G46" s="13" t="s">
         <v>6</v>
@@ -2676,23 +2690,23 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="14">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>81</v>
+      </c>
+      <c r="F47" s="24" t="s">
         <v>62</v>
-      </c>
-      <c r="B47" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="14">
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
-        <v>95</v>
-      </c>
-      <c r="F47" s="24" t="s">
-        <v>76</v>
       </c>
       <c r="G47" s="13" t="s">
         <v>7</v>
@@ -2702,23 +2716,23 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" s="14">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>81</v>
+      </c>
+      <c r="F48" s="24" t="s">
         <v>62</v>
-      </c>
-      <c r="B48" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D48" s="14">
-        <v>1</v>
-      </c>
-      <c r="E48" t="s">
-        <v>95</v>
-      </c>
-      <c r="F48" s="24" t="s">
-        <v>76</v>
       </c>
       <c r="G48" s="13" t="s">
         <v>29</v>
@@ -2738,23 +2752,23 @@
       <c r="H49" s="13"/>
     </row>
     <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" s="14">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>82</v>
+      </c>
+      <c r="F50" s="24" t="s">
         <v>63</v>
-      </c>
-      <c r="B50" t="s">
-        <v>88</v>
-      </c>
-      <c r="C50" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D50" s="14">
-        <v>1</v>
-      </c>
-      <c r="E50" t="s">
-        <v>96</v>
-      </c>
-      <c r="F50" s="24" t="s">
-        <v>77</v>
       </c>
       <c r="G50" s="13" t="s">
         <v>5</v>
@@ -2767,23 +2781,23 @@
       </c>
     </row>
     <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" s="14">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>82</v>
+      </c>
+      <c r="F51" s="24" t="s">
         <v>63</v>
-      </c>
-      <c r="B51" t="s">
-        <v>88</v>
-      </c>
-      <c r="C51" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D51" s="14">
-        <v>1</v>
-      </c>
-      <c r="E51" t="s">
-        <v>96</v>
-      </c>
-      <c r="F51" s="24" t="s">
-        <v>77</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>6</v>
@@ -2793,23 +2807,23 @@
       </c>
     </row>
     <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D52" s="14">
+        <v>1</v>
+      </c>
+      <c r="E52" t="s">
+        <v>82</v>
+      </c>
+      <c r="F52" s="24" t="s">
         <v>63</v>
-      </c>
-      <c r="B52" t="s">
-        <v>88</v>
-      </c>
-      <c r="C52" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D52" s="14">
-        <v>1</v>
-      </c>
-      <c r="E52" t="s">
-        <v>96</v>
-      </c>
-      <c r="F52" s="24" t="s">
-        <v>77</v>
       </c>
       <c r="G52" s="13" t="s">
         <v>7</v>
@@ -2819,23 +2833,23 @@
       </c>
     </row>
     <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B53" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" s="14">
+        <v>1</v>
+      </c>
+      <c r="E53" t="s">
+        <v>82</v>
+      </c>
+      <c r="F53" s="24" t="s">
         <v>63</v>
-      </c>
-      <c r="B53" t="s">
-        <v>88</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D53" s="14">
-        <v>1</v>
-      </c>
-      <c r="E53" t="s">
-        <v>96</v>
-      </c>
-      <c r="F53" s="24" t="s">
-        <v>77</v>
       </c>
       <c r="G53" s="13" t="s">
         <v>29</v>
@@ -2855,23 +2869,23 @@
       <c r="H54" s="13"/>
     </row>
     <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B55" t="s">
+        <v>74</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D55" s="14">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
+        <v>83</v>
+      </c>
+      <c r="F55" s="24" t="s">
         <v>64</v>
-      </c>
-      <c r="B55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D55" s="14">
-        <v>1</v>
-      </c>
-      <c r="E55" t="s">
-        <v>97</v>
-      </c>
-      <c r="F55" s="24" t="s">
-        <v>78</v>
       </c>
       <c r="G55" s="13" t="s">
         <v>5</v>
@@ -2884,23 +2898,23 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D56" s="14">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>83</v>
+      </c>
+      <c r="F56" s="24" t="s">
         <v>64</v>
-      </c>
-      <c r="B56" t="s">
-        <v>88</v>
-      </c>
-      <c r="C56" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D56" s="14">
-        <v>1</v>
-      </c>
-      <c r="E56" t="s">
-        <v>97</v>
-      </c>
-      <c r="F56" s="24" t="s">
-        <v>78</v>
       </c>
       <c r="G56" s="13" t="s">
         <v>6</v>
@@ -2910,23 +2924,23 @@
       </c>
     </row>
     <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" t="s">
+        <v>74</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="14">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
+        <v>83</v>
+      </c>
+      <c r="F57" s="24" t="s">
         <v>64</v>
-      </c>
-      <c r="B57" t="s">
-        <v>88</v>
-      </c>
-      <c r="C57" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D57" s="14">
-        <v>1</v>
-      </c>
-      <c r="E57" t="s">
-        <v>97</v>
-      </c>
-      <c r="F57" s="24" t="s">
-        <v>78</v>
       </c>
       <c r="G57" s="13" t="s">
         <v>7</v>
@@ -2936,23 +2950,23 @@
       </c>
     </row>
     <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B58" t="s">
+        <v>74</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D58" s="14">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>83</v>
+      </c>
+      <c r="F58" s="24" t="s">
         <v>64</v>
-      </c>
-      <c r="B58" t="s">
-        <v>88</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D58" s="14">
-        <v>1</v>
-      </c>
-      <c r="E58" t="s">
-        <v>97</v>
-      </c>
-      <c r="F58" s="24" t="s">
-        <v>78</v>
       </c>
       <c r="G58" s="13" t="s">
         <v>29</v>
@@ -2972,23 +2986,23 @@
       <c r="H59" s="13"/>
     </row>
     <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60" s="14">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
+        <v>84</v>
+      </c>
+      <c r="F60" s="24" t="s">
         <v>65</v>
-      </c>
-      <c r="B60" t="s">
-        <v>88</v>
-      </c>
-      <c r="C60" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D60" s="14">
-        <v>1</v>
-      </c>
-      <c r="E60" t="s">
-        <v>98</v>
-      </c>
-      <c r="F60" s="24" t="s">
-        <v>79</v>
       </c>
       <c r="G60" s="13" t="s">
         <v>5</v>
@@ -3001,23 +3015,23 @@
       </c>
     </row>
     <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D61" s="14">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>84</v>
+      </c>
+      <c r="F61" s="24" t="s">
         <v>65</v>
-      </c>
-      <c r="B61" t="s">
-        <v>88</v>
-      </c>
-      <c r="C61" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D61" s="14">
-        <v>1</v>
-      </c>
-      <c r="E61" t="s">
-        <v>98</v>
-      </c>
-      <c r="F61" s="24" t="s">
-        <v>79</v>
       </c>
       <c r="G61" s="13" t="s">
         <v>6</v>
@@ -3027,23 +3041,23 @@
       </c>
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+      <c r="A62" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D62" s="14">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
+        <v>84</v>
+      </c>
+      <c r="F62" s="24" t="s">
         <v>65</v>
-      </c>
-      <c r="B62" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D62" s="14">
-        <v>1</v>
-      </c>
-      <c r="E62" t="s">
-        <v>98</v>
-      </c>
-      <c r="F62" s="24" t="s">
-        <v>79</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>7</v>
@@ -3053,23 +3067,23 @@
       </c>
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B63" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63" s="14">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
+        <v>84</v>
+      </c>
+      <c r="F63" s="24" t="s">
         <v>65</v>
-      </c>
-      <c r="B63" t="s">
-        <v>88</v>
-      </c>
-      <c r="C63" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D63" s="14">
-        <v>1</v>
-      </c>
-      <c r="E63" t="s">
-        <v>98</v>
-      </c>
-      <c r="F63" s="24" t="s">
-        <v>79</v>
       </c>
       <c r="G63" s="13" t="s">
         <v>29</v>
@@ -3088,24 +3102,24 @@
       <c r="G64" s="13"/>
       <c r="H64" s="13"/>
     </row>
-    <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
+    <row r="65" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B65" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D65" s="14">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
+        <v>85</v>
+      </c>
+      <c r="F65" s="24" t="s">
         <v>66</v>
-      </c>
-      <c r="B65" t="s">
-        <v>88</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D65" s="14">
-        <v>1</v>
-      </c>
-      <c r="E65" t="s">
-        <v>99</v>
-      </c>
-      <c r="F65" s="24" t="s">
-        <v>80</v>
       </c>
       <c r="G65" s="13" t="s">
         <v>5</v>
@@ -3117,24 +3131,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
+    <row r="66" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B66" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D66" s="14">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
+        <v>85</v>
+      </c>
+      <c r="F66" s="24" t="s">
         <v>66</v>
-      </c>
-      <c r="B66" t="s">
-        <v>88</v>
-      </c>
-      <c r="C66" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D66" s="14">
-        <v>1</v>
-      </c>
-      <c r="E66" t="s">
-        <v>99</v>
-      </c>
-      <c r="F66" s="24" t="s">
-        <v>80</v>
       </c>
       <c r="G66" s="13" t="s">
         <v>6</v>
@@ -3143,24 +3157,24 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="s">
+    <row r="67" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B67" t="s">
+        <v>74</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D67" s="14">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>85</v>
+      </c>
+      <c r="F67" s="24" t="s">
         <v>66</v>
-      </c>
-      <c r="B67" t="s">
-        <v>88</v>
-      </c>
-      <c r="C67" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D67" s="14">
-        <v>1</v>
-      </c>
-      <c r="E67" t="s">
-        <v>99</v>
-      </c>
-      <c r="F67" s="24" t="s">
-        <v>80</v>
       </c>
       <c r="G67" s="13" t="s">
         <v>7</v>
@@ -3169,24 +3183,24 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="13" t="s">
+    <row r="68" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B68" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D68" s="14">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>85</v>
+      </c>
+      <c r="F68" s="24" t="s">
         <v>66</v>
-      </c>
-      <c r="B68" t="s">
-        <v>88</v>
-      </c>
-      <c r="C68" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D68" s="14">
-        <v>1</v>
-      </c>
-      <c r="E68" t="s">
-        <v>99</v>
-      </c>
-      <c r="F68" s="24" t="s">
-        <v>80</v>
       </c>
       <c r="G68" s="13" t="s">
         <v>29</v>
@@ -3195,7 +3209,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="13"/>
       <c r="B69"/>
       <c r="C69" s="13"/>
@@ -3205,24 +3219,24 @@
       <c r="G69" s="13"/>
       <c r="H69" s="13"/>
     </row>
-    <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="13" t="s">
+    <row r="70" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B70" t="s">
+        <v>74</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D70" s="14">
+        <v>1</v>
+      </c>
+      <c r="E70" t="s">
+        <v>86</v>
+      </c>
+      <c r="F70" s="24" t="s">
         <v>67</v>
-      </c>
-      <c r="B70" t="s">
-        <v>88</v>
-      </c>
-      <c r="C70" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D70" s="14">
-        <v>1</v>
-      </c>
-      <c r="E70" t="s">
-        <v>100</v>
-      </c>
-      <c r="F70" s="24" t="s">
-        <v>81</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>5</v>
@@ -3234,24 +3248,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="13" t="s">
+    <row r="71" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B71" t="s">
+        <v>74</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D71" s="14">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>86</v>
+      </c>
+      <c r="F71" s="24" t="s">
         <v>67</v>
-      </c>
-      <c r="B71" t="s">
-        <v>88</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D71" s="14">
-        <v>1</v>
-      </c>
-      <c r="E71" t="s">
-        <v>100</v>
-      </c>
-      <c r="F71" s="24" t="s">
-        <v>81</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>6</v>
@@ -3260,24 +3274,24 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
+    <row r="72" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B72" t="s">
+        <v>74</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D72" s="14">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
+        <v>86</v>
+      </c>
+      <c r="F72" s="24" t="s">
         <v>67</v>
-      </c>
-      <c r="B72" t="s">
-        <v>88</v>
-      </c>
-      <c r="C72" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D72" s="14">
-        <v>1</v>
-      </c>
-      <c r="E72" t="s">
-        <v>100</v>
-      </c>
-      <c r="F72" s="24" t="s">
-        <v>81</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>7</v>
@@ -3286,24 +3300,24 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="13" t="s">
+    <row r="73" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B73" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D73" s="14">
+        <v>1</v>
+      </c>
+      <c r="E73" t="s">
+        <v>86</v>
+      </c>
+      <c r="F73" s="24" t="s">
         <v>67</v>
-      </c>
-      <c r="B73" t="s">
-        <v>88</v>
-      </c>
-      <c r="C73" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D73" s="14">
-        <v>1</v>
-      </c>
-      <c r="E73" t="s">
-        <v>100</v>
-      </c>
-      <c r="F73" s="24" t="s">
-        <v>81</v>
       </c>
       <c r="G73" s="13" t="s">
         <v>29</v>
@@ -3312,7 +3326,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="13"/>
       <c r="B74"/>
       <c r="C74" s="13"/>
@@ -3322,24 +3336,24 @@
       <c r="G74" s="13"/>
       <c r="H74" s="13"/>
     </row>
-    <row r="75" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="13" t="s">
+    <row r="75" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B75" t="s">
+        <v>74</v>
+      </c>
+      <c r="C75" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D75" s="14">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
+        <v>87</v>
+      </c>
+      <c r="F75" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="B75" t="s">
-        <v>88</v>
-      </c>
-      <c r="C75" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D75" s="14">
-        <v>1</v>
-      </c>
-      <c r="E75" t="s">
-        <v>101</v>
-      </c>
-      <c r="F75" s="24" t="s">
-        <v>82</v>
       </c>
       <c r="G75" s="13" t="s">
         <v>5</v>
@@ -3351,24 +3365,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="13" t="s">
+    <row r="76" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B76" t="s">
+        <v>74</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D76" s="14">
+        <v>1</v>
+      </c>
+      <c r="E76" t="s">
+        <v>87</v>
+      </c>
+      <c r="F76" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="B76" t="s">
-        <v>88</v>
-      </c>
-      <c r="C76" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D76" s="14">
-        <v>1</v>
-      </c>
-      <c r="E76" t="s">
-        <v>101</v>
-      </c>
-      <c r="F76" s="24" t="s">
-        <v>82</v>
       </c>
       <c r="G76" s="13" t="s">
         <v>6</v>
@@ -3377,24 +3391,24 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="13" t="s">
+    <row r="77" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B77" t="s">
+        <v>74</v>
+      </c>
+      <c r="C77" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D77" s="14">
+        <v>1</v>
+      </c>
+      <c r="E77" t="s">
+        <v>87</v>
+      </c>
+      <c r="F77" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="B77" t="s">
-        <v>88</v>
-      </c>
-      <c r="C77" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D77" s="14">
-        <v>1</v>
-      </c>
-      <c r="E77" t="s">
-        <v>101</v>
-      </c>
-      <c r="F77" s="24" t="s">
-        <v>82</v>
       </c>
       <c r="G77" s="13" t="s">
         <v>7</v>
@@ -3403,24 +3417,24 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="13" t="s">
+    <row r="78" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B78" t="s">
+        <v>74</v>
+      </c>
+      <c r="C78" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D78" s="14">
+        <v>1</v>
+      </c>
+      <c r="E78" t="s">
+        <v>87</v>
+      </c>
+      <c r="F78" s="24" t="s">
         <v>68</v>
-      </c>
-      <c r="B78" t="s">
-        <v>88</v>
-      </c>
-      <c r="C78" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D78" s="14">
-        <v>1</v>
-      </c>
-      <c r="E78" t="s">
-        <v>101</v>
-      </c>
-      <c r="F78" s="24" t="s">
-        <v>82</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>29</v>
@@ -3429,7 +3443,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="13"/>
       <c r="B79"/>
       <c r="C79" s="13"/>
@@ -3439,24 +3453,24 @@
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
     </row>
-    <row r="80" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="13" t="s">
+    <row r="80" spans="1:12" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B80" t="s">
+        <v>74</v>
+      </c>
+      <c r="C80" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D80" s="15">
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
+        <v>88</v>
+      </c>
+      <c r="F80" s="25" t="s">
         <v>69</v>
-      </c>
-      <c r="B80" t="s">
-        <v>88</v>
-      </c>
-      <c r="C80" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D80" s="15">
-        <v>1</v>
-      </c>
-      <c r="E80" t="s">
-        <v>102</v>
-      </c>
-      <c r="F80" s="25" t="s">
-        <v>83</v>
       </c>
       <c r="G80" s="16" t="s">
         <v>5</v>
@@ -3467,25 +3481,26 @@
       <c r="I80" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="13" t="s">
+      <c r="L80" s="2"/>
+    </row>
+    <row r="81" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B81" t="s">
+        <v>74</v>
+      </c>
+      <c r="C81" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D81" s="14">
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
+        <v>88</v>
+      </c>
+      <c r="F81" s="24" t="s">
         <v>69</v>
-      </c>
-      <c r="B81" t="s">
-        <v>88</v>
-      </c>
-      <c r="C81" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D81" s="14">
-        <v>1</v>
-      </c>
-      <c r="E81" t="s">
-        <v>102</v>
-      </c>
-      <c r="F81" s="24" t="s">
-        <v>83</v>
       </c>
       <c r="G81" s="13" t="s">
         <v>6</v>
@@ -3494,24 +3509,24 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="13" t="s">
+    <row r="82" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B82" t="s">
+        <v>74</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D82" s="14">
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
+        <v>88</v>
+      </c>
+      <c r="F82" s="24" t="s">
         <v>69</v>
-      </c>
-      <c r="B82" t="s">
-        <v>88</v>
-      </c>
-      <c r="C82" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D82" s="14">
-        <v>1</v>
-      </c>
-      <c r="E82" t="s">
-        <v>102</v>
-      </c>
-      <c r="F82" s="24" t="s">
-        <v>83</v>
       </c>
       <c r="G82" s="13" t="s">
         <v>7</v>
@@ -3520,24 +3535,24 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="13" t="s">
+    <row r="83" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B83" t="s">
+        <v>74</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D83" s="14">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>88</v>
+      </c>
+      <c r="F83" s="24" t="s">
         <v>69</v>
-      </c>
-      <c r="B83" t="s">
-        <v>88</v>
-      </c>
-      <c r="C83" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D83" s="14">
-        <v>1</v>
-      </c>
-      <c r="E83" t="s">
-        <v>102</v>
-      </c>
-      <c r="F83" s="24" t="s">
-        <v>83</v>
       </c>
       <c r="G83" s="13" t="s">
         <v>29</v>
@@ -3546,7 +3561,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="13"/>
       <c r="B84"/>
       <c r="C84" s="13"/>
@@ -3556,24 +3571,24 @@
       <c r="G84" s="13"/>
       <c r="H84" s="13"/>
     </row>
-    <row r="85" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="13" t="s">
+    <row r="85" spans="1:12" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B85" t="s">
+        <v>74</v>
+      </c>
+      <c r="C85" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D85" s="15">
+        <v>1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>89</v>
+      </c>
+      <c r="F85" s="24" t="s">
         <v>70</v>
-      </c>
-      <c r="B85" t="s">
-        <v>88</v>
-      </c>
-      <c r="C85" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D85" s="15">
-        <v>1</v>
-      </c>
-      <c r="E85" t="s">
-        <v>103</v>
-      </c>
-      <c r="F85" s="24" t="s">
-        <v>84</v>
       </c>
       <c r="G85" s="16" t="s">
         <v>5</v>
@@ -3584,25 +3599,26 @@
       <c r="I85" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="13" t="s">
+      <c r="L85" s="2"/>
+    </row>
+    <row r="86" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B86" t="s">
+        <v>74</v>
+      </c>
+      <c r="C86" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D86" s="14">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>89</v>
+      </c>
+      <c r="F86" s="24" t="s">
         <v>70</v>
-      </c>
-      <c r="B86" t="s">
-        <v>88</v>
-      </c>
-      <c r="C86" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D86" s="14">
-        <v>1</v>
-      </c>
-      <c r="E86" t="s">
-        <v>103</v>
-      </c>
-      <c r="F86" s="24" t="s">
-        <v>84</v>
       </c>
       <c r="G86" s="13" t="s">
         <v>6</v>
@@ -3611,24 +3627,24 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="13" t="s">
+    <row r="87" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B87" t="s">
+        <v>74</v>
+      </c>
+      <c r="C87" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D87" s="14">
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>89</v>
+      </c>
+      <c r="F87" s="24" t="s">
         <v>70</v>
-      </c>
-      <c r="B87" t="s">
-        <v>88</v>
-      </c>
-      <c r="C87" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D87" s="14">
-        <v>1</v>
-      </c>
-      <c r="E87" t="s">
-        <v>103</v>
-      </c>
-      <c r="F87" s="24" t="s">
-        <v>84</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>7</v>
@@ -3637,24 +3653,24 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="13" t="s">
+    <row r="88" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B88" t="s">
+        <v>74</v>
+      </c>
+      <c r="C88" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D88" s="14">
+        <v>1</v>
+      </c>
+      <c r="E88" t="s">
+        <v>89</v>
+      </c>
+      <c r="F88" s="24" t="s">
         <v>70</v>
-      </c>
-      <c r="B88" t="s">
-        <v>88</v>
-      </c>
-      <c r="C88" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D88" s="14">
-        <v>1</v>
-      </c>
-      <c r="E88" t="s">
-        <v>103</v>
-      </c>
-      <c r="F88" s="24" t="s">
-        <v>84</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>29</v>
@@ -3663,7 +3679,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="13"/>
       <c r="B89"/>
       <c r="C89" s="13"/>
@@ -3673,24 +3689,24 @@
       <c r="G89" s="13"/>
       <c r="H89" s="13"/>
     </row>
-    <row r="90" spans="1:9" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="13" t="s">
+    <row r="90" spans="1:12" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B90" t="s">
+        <v>74</v>
+      </c>
+      <c r="C90" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D90" s="15">
+        <v>1</v>
+      </c>
+      <c r="E90" t="s">
+        <v>90</v>
+      </c>
+      <c r="F90" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="B90" t="s">
-        <v>88</v>
-      </c>
-      <c r="C90" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D90" s="15">
-        <v>1</v>
-      </c>
-      <c r="E90" t="s">
-        <v>104</v>
-      </c>
-      <c r="F90" s="25" t="s">
-        <v>85</v>
       </c>
       <c r="G90" s="16" t="s">
         <v>5</v>
@@ -3701,25 +3717,26 @@
       <c r="I90" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="13" t="s">
+      <c r="L90" s="2"/>
+    </row>
+    <row r="91" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B91" t="s">
+        <v>74</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D91" s="14">
+        <v>1</v>
+      </c>
+      <c r="E91" t="s">
+        <v>90</v>
+      </c>
+      <c r="F91" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="B91" t="s">
-        <v>88</v>
-      </c>
-      <c r="C91" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D91" s="14">
-        <v>1</v>
-      </c>
-      <c r="E91" t="s">
-        <v>104</v>
-      </c>
-      <c r="F91" s="25" t="s">
-        <v>85</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>6</v>
@@ -3728,24 +3745,24 @@
         <v>-54.105166666666669</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="13" t="s">
+    <row r="92" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B92" t="s">
+        <v>74</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D92" s="14">
+        <v>1</v>
+      </c>
+      <c r="E92" t="s">
+        <v>90</v>
+      </c>
+      <c r="F92" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="B92" t="s">
-        <v>88</v>
-      </c>
-      <c r="C92" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D92" s="14">
-        <v>1</v>
-      </c>
-      <c r="E92" t="s">
-        <v>104</v>
-      </c>
-      <c r="F92" s="25" t="s">
-        <v>85</v>
       </c>
       <c r="G92" s="13" t="s">
         <v>7</v>
@@ -3754,24 +3771,24 @@
         <v>-89.65361</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="13" t="s">
+    <row r="93" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B93" t="s">
+        <v>74</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D93" s="14">
+        <v>1</v>
+      </c>
+      <c r="E93" t="s">
+        <v>90</v>
+      </c>
+      <c r="F93" s="25" t="s">
         <v>71</v>
-      </c>
-      <c r="B93" t="s">
-        <v>88</v>
-      </c>
-      <c r="C93" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D93" s="14">
-        <v>1</v>
-      </c>
-      <c r="E93" t="s">
-        <v>104</v>
-      </c>
-      <c r="F93" s="25" t="s">
-        <v>85</v>
       </c>
       <c r="G93" s="13" t="s">
         <v>29</v>
@@ -3780,7 +3797,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="13"/>
       <c r="B94"/>
       <c r="C94" s="13"/>
@@ -3790,12 +3807,12 @@
       <c r="G94" s="13"/>
       <c r="H94" s="13"/>
     </row>
-    <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="13" t="s">
-        <v>50</v>
+    <row r="95" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B95" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C95" s="13" t="s">
         <v>47</v>
@@ -3803,23 +3820,37 @@
       <c r="D95" s="14">
         <v>1</v>
       </c>
-      <c r="E95" s="14"/>
+      <c r="E95" t="s">
+        <v>107</v>
+      </c>
       <c r="F95" s="20" t="s">
-        <v>55</v>
+        <v>106</v>
       </c>
       <c r="G95" s="13"/>
       <c r="H95" s="13"/>
       <c r="I95" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="13"/>
-      <c r="B96" s="13"/>
-      <c r="C96" s="13"/>
-      <c r="D96" s="14"/>
-      <c r="E96" s="14"/>
-      <c r="F96" s="13"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B96" t="s">
+        <v>74</v>
+      </c>
+      <c r="C96" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D96" s="14">
+        <v>1</v>
+      </c>
+      <c r="E96" t="s">
+        <v>108</v>
+      </c>
+      <c r="F96" s="13" t="s">
+        <v>105</v>
+      </c>
       <c r="G96" s="13"/>
       <c r="H96" s="13"/>
     </row>

</xml_diff>

<commit_message>
Southern Ocean - fixed deployment dates
Fixed deployment dates based on cruise reports and WHOI documentation
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_GS03FLMA_00001.xlsx
+++ b/deployment/Omaha_Cal_Info_GS03FLMA_00001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="460" windowWidth="25360" windowHeight="15820" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="32320" windowHeight="17340"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -1397,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1478,7 +1478,7 @@
         <v>0.99652777777777779</v>
       </c>
       <c r="G2" s="7">
-        <v>42345</v>
+        <v>42356</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>50</v>
@@ -1522,7 +1522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>

</xml_diff>